<commit_message>
0.0.4: Generic of primitives are ignored. fixed.
</commit_message>
<xml_diff>
--- a/meta/components/ComponentSample.xlsx
+++ b/meta/components/ComponentSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8950B911-30ED-EE4D-AE99-0E58DF0FC4E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36DAB36-CACC-1040-AEAC-B21745B4566A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t>パッケージ</t>
   </si>
@@ -606,6 +606,18 @@
   </si>
   <si>
     <t>@</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop05</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop06</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>integer</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1362,6 +1374,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1375,24 +1405,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1808,7 +1820,7 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1898,10 +1910,10 @@
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="88"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="10"/>
       <c r="D9" s="33"/>
       <c r="E9" s="11"/>
@@ -1912,10 +1924,10 @@
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="10"/>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
@@ -1926,10 +1938,10 @@
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="88"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
@@ -1942,10 +1954,10 @@
       <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="88"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="86" t="s">
         <v>80</v>
       </c>
@@ -1962,11 +1974,11 @@
         <v>1</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="65"/>
       <c r="G13" s="65"/>
       <c r="H13" s="34"/>
@@ -2066,10 +2078,10 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="93"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="64"/>
       <c r="D20" t="s">
         <v>36</v>
@@ -2094,10 +2106,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:12" s="32" customFormat="1">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="93"/>
+      <c r="B22" s="88"/>
       <c r="C22" s="64" t="s">
         <v>15</v>
       </c>
@@ -2433,45 +2445,45 @@
       <c r="L43" s="15"/>
     </row>
     <row r="44" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A44" s="95" t="s">
+      <c r="A44" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="95" t="s">
+      <c r="B44" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="94" t="s">
+      <c r="C44" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="94" t="s">
+      <c r="D44" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="94" t="s">
+      <c r="E44" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="96" t="s">
+      <c r="F44" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="G44" s="96" t="s">
+      <c r="G44" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="94" t="s">
+      <c r="H44" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="94"/>
+      <c r="I44" s="89"/>
       <c r="J44" s="16"/>
       <c r="K44" s="17"/>
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="95"/>
-      <c r="B45" s="95"/>
-      <c r="C45" s="94"/>
-      <c r="D45" s="94"/>
-      <c r="E45" s="94"/>
-      <c r="F45" s="97"/>
-      <c r="G45" s="97"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="94"/>
+      <c r="A45" s="90"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="89"/>
       <c r="J45" s="18"/>
       <c r="K45" s="29"/>
       <c r="L45" s="15"/>
@@ -2584,12 +2596,20 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B50" s="73"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="20"/>
+      <c r="B50" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="69"/>
+      <c r="G50" s="69" t="s">
+        <v>15</v>
+      </c>
       <c r="H50" s="20"/>
       <c r="I50" s="21"/>
       <c r="J50" s="21"/>
@@ -2601,12 +2621,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B51" s="73"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="74"/>
+      <c r="B51" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="E51" s="74"/>
       <c r="F51" s="74"/>
-      <c r="G51" s="75"/>
+      <c r="G51" s="75" t="s">
+        <v>15</v>
+      </c>
       <c r="H51" s="74"/>
       <c r="I51" s="76"/>
       <c r="J51" s="76"/>
@@ -2816,6 +2844,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H44:I45"/>
@@ -2826,11 +2859,6 @@
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="G44:G45"/>
     <mergeCell ref="F44:F45"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">

</xml_diff>

<commit_message>
0.0.5: Use basedir of objects for property import statements instead of component.
</commit_message>
<xml_diff>
--- a/meta/components/ComponentSample.xlsx
+++ b/meta/components/ComponentSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36DAB36-CACC-1040-AEAC-B21745B4566A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269FA8D9-4432-C740-A027-E2FD37D6BF62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,10 +185,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>%</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Labels Class for i18n</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -618,6 +614,10 @@
   </si>
   <si>
     <t>integer</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>%%</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1374,6 +1374,21 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1390,21 +1405,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1819,8 +1819,8 @@
   </sheetPr>
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1838,7 +1838,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1846,17 +1846,17 @@
     </row>
     <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1867,27 +1867,27 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
       <c r="F6" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="11"/>
@@ -1910,61 +1910,61 @@
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="93" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="94"/>
+      <c r="A9" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="88"/>
       <c r="C9" s="10"/>
       <c r="D9" s="33"/>
       <c r="E9" s="11"/>
       <c r="F9" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="93" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="94"/>
+      <c r="A10" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="88"/>
       <c r="C10" s="10"/>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
       <c r="F10" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="94"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="10" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
       <c r="F11" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="93" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="94"/>
+      <c r="A12" s="87" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="88"/>
       <c r="C12" s="86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="11"/>
       <c r="F12" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="35"/>
@@ -1974,11 +1974,11 @@
         <v>1</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="95" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
+      <c r="C13" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="90"/>
+      <c r="E13" s="91"/>
       <c r="F13" s="65"/>
       <c r="G13" s="65"/>
       <c r="H13" s="34"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="8"/>
@@ -2003,14 +2003,14 @@
     </row>
     <row r="15" spans="1:10" s="32" customFormat="1">
       <c r="A15" s="62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="63"/>
       <c r="C15" s="64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
@@ -2019,12 +2019,12 @@
     </row>
     <row r="16" spans="1:10" s="32" customFormat="1">
       <c r="A16" s="62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="63"/>
       <c r="C16" s="64"/>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
@@ -2033,12 +2033,12 @@
     </row>
     <row r="17" spans="1:12" s="32" customFormat="1">
       <c r="A17" s="62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="63"/>
       <c r="C17" s="64"/>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
@@ -2047,14 +2047,14 @@
     </row>
     <row r="18" spans="1:12" s="32" customFormat="1">
       <c r="A18" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="63"/>
       <c r="C18" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -2063,14 +2063,14 @@
     </row>
     <row r="19" spans="1:12" s="32" customFormat="1">
       <c r="A19" s="62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -2078,13 +2078,13 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="87" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="88"/>
+      <c r="A20" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="93"/>
       <c r="C20" s="64"/>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -2106,10 +2106,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:12" s="32" customFormat="1">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="88"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="64" t="s">
         <v>15</v>
       </c>
@@ -2135,14 +2135,14 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
       <c r="E24" s="81"/>
       <c r="F24" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
@@ -2174,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -2228,14 +2228,14 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
       <c r="E30" s="81"/>
       <c r="F30" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
@@ -2317,14 +2317,14 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="81"/>
       <c r="F36" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G36" s="44"/>
       <c r="H36" s="44"/>
@@ -2338,7 +2338,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" s="42"/>
       <c r="D37" s="42"/>
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
@@ -2374,7 +2374,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="40"/>
       <c r="D39" s="40"/>
@@ -2418,7 +2418,7 @@
     <row r="42" spans="1:12">
       <c r="A42" s="13"/>
       <c r="B42" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2445,45 +2445,45 @@
       <c r="L43" s="15"/>
     </row>
     <row r="44" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="90" t="s">
+      <c r="B44" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="89" t="s">
+      <c r="C44" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="89" t="s">
+      <c r="D44" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="89" t="s">
+      <c r="E44" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="G44" s="91" t="s">
+      <c r="F44" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="G44" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="89" t="s">
+      <c r="H44" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="89"/>
+      <c r="I44" s="94"/>
       <c r="J44" s="16"/>
       <c r="K44" s="17"/>
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="90"/>
-      <c r="B45" s="90"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
+      <c r="A45" s="95"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="94"/>
       <c r="J45" s="18"/>
       <c r="K45" s="29"/>
       <c r="L45" s="15"/>
@@ -2493,21 +2493,21 @@
         <v>1</v>
       </c>
       <c r="B46" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="78" t="s">
         <v>57</v>
-      </c>
-      <c r="C46" s="78" t="s">
-        <v>58</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>15</v>
       </c>
       <c r="G46" s="69"/>
       <c r="H46" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
@@ -2520,10 +2520,10 @@
         <v>2</v>
       </c>
       <c r="B47" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="78" t="s">
         <v>60</v>
-      </c>
-      <c r="C47" s="78" t="s">
-        <v>61</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20" t="b">
@@ -2532,7 +2532,7 @@
       <c r="F47" s="20"/>
       <c r="G47" s="69"/>
       <c r="H47" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I47" s="21"/>
       <c r="J47" s="21"/>
@@ -2545,13 +2545,13 @@
         <v>3</v>
       </c>
       <c r="B48" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="79" t="s">
+      <c r="D48" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="20"/>
@@ -2559,7 +2559,7 @@
         <v>15</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I48" s="21"/>
       <c r="J48" s="21"/>
@@ -2572,10 +2572,10 @@
         <v>4</v>
       </c>
       <c r="B49" s="73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
@@ -2584,7 +2584,7 @@
         <v>15</v>
       </c>
       <c r="H49" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I49" s="21"/>
       <c r="J49" s="21"/>
@@ -2597,13 +2597,13 @@
         <v>5</v>
       </c>
       <c r="B50" s="73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="80" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
@@ -2622,13 +2622,13 @@
         <v>6</v>
       </c>
       <c r="B51" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="C51" s="80" t="s">
-        <v>64</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>83</v>
       </c>
       <c r="E51" s="74"/>
       <c r="F51" s="74"/>
@@ -2844,11 +2844,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:E13"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H44:I45"/>
@@ -2859,6 +2854,11 @@
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="G44:G45"/>
     <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
@@ -2930,10 +2930,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="56" t="s">
         <v>11</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="B4" s="57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>14</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="B5" s="59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="60"/>
       <c r="F5" s="60" t="s">

</xml_diff>